<commit_message>
pass targetTable in to CreateDestinationTable, load each worksheet if the xlsx file has more than one
</commit_message>
<xml_diff>
--- a/BulkInsert/alphabet.xlsx
+++ b/BulkInsert/alphabet.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr\source\repos\bulkinsert\BulkInsert\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{96507C0F-1E3E-4763-8E6C-0C6BC34BE628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247E8B9D-0FC2-45E0-8F4D-81EF36316602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1764" yWindow="-21300" windowWidth="23040" windowHeight="13560"/>
+    <workbookView xWindow="-7224" yWindow="-26028" windowWidth="46296" windowHeight="25536" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet.-name test" sheetId="1" r:id="rId1"/>
+    <sheet name="alphabet" sheetId="1" r:id="rId1"/>
+    <sheet name="primes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Id</t>
   </si>
@@ -104,12 +105,15 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>PrimeNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -943,16 +947,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,7 +964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -968,7 +972,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -976,7 +980,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -984,7 +988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -992,7 +996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1000,7 +1004,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1016,7 +1020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1024,7 +1028,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1040,7 +1044,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1056,7 +1060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1064,7 +1068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1088,7 +1092,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1096,7 +1100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1112,7 +1116,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1120,7 +1124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1128,7 +1132,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1136,7 +1140,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1152,7 +1156,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1160,12 +1164,126 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA672CC-B4EA-48F2-9012-70C590E53B76}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>